<commit_message>
sorting files into folders
</commit_message>
<xml_diff>
--- a/Notebooks/Angel/quandl_country_list.xlsx
+++ b/Notebooks/Angel/quandl_country_list.xlsx
@@ -3,24 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_F25DC773A252ABEACE02EC449B5978485ADE58AD" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{188E9992-2DE9-41F2-9482-CF1ECDAFD659}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_F25DC773A252ABEACE02EC449B5978485ADE58AD" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{2E146155-CA5E-4180-A6AB-AB2F6B5C69E7}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="2210" windowWidth="14400" windowHeight="7460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22395" yWindow="-9210" windowWidth="14400" windowHeight="7455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="391">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -1190,6 +1196,9 @@
   </si>
   <si>
     <t>ZWE</t>
+  </si>
+  <si>
+    <t>UNAE/GVAKD_</t>
   </si>
 </sst>
 </file>
@@ -1512,14 +1521,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
-      <selection activeCell="E192" sqref="E192"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="H164" sqref="H164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -1529,6 +1540,13 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1" t="str">
+        <f>C1&amp;+B1</f>
+        <v>UNAE/GVAKD_AFG</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
@@ -1539,6 +1557,13 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>390</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D65" si="0">C2&amp;+B2</f>
+        <v>UNAE/GVAKD_ALB</v>
+      </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
     </row>
@@ -1549,6 +1574,13 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_DZA</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
@@ -1559,6 +1591,13 @@
       <c r="B4" t="s">
         <v>7</v>
       </c>
+      <c r="C4" t="s">
+        <v>390</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_AND</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
@@ -1569,6 +1608,13 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>390</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_AGO</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
@@ -1579,6 +1625,13 @@
       <c r="B6" t="s">
         <v>11</v>
       </c>
+      <c r="C6" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_ATG</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
@@ -1589,6 +1642,13 @@
       <c r="B7" t="s">
         <v>13</v>
       </c>
+      <c r="C7" t="s">
+        <v>390</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_ARG</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
@@ -1599,6 +1659,13 @@
       <c r="B8" t="s">
         <v>15</v>
       </c>
+      <c r="C8" t="s">
+        <v>390</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_ARM</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
@@ -1609,6 +1676,13 @@
       <c r="B9" t="s">
         <v>17</v>
       </c>
+      <c r="C9" t="s">
+        <v>390</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_AUS</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
@@ -1619,6 +1693,13 @@
       <c r="B10" t="s">
         <v>19</v>
       </c>
+      <c r="C10" t="s">
+        <v>390</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_AUT</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
@@ -1629,6 +1710,13 @@
       <c r="B11" t="s">
         <v>21</v>
       </c>
+      <c r="C11" t="s">
+        <v>390</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_AZE</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
@@ -1639,6 +1727,13 @@
       <c r="B12" t="s">
         <v>23</v>
       </c>
+      <c r="C12" t="s">
+        <v>390</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BHS</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
@@ -1649,6 +1744,13 @@
       <c r="B13" t="s">
         <v>25</v>
       </c>
+      <c r="C13" t="s">
+        <v>390</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BHR</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
@@ -1659,6 +1761,13 @@
       <c r="B14" t="s">
         <v>27</v>
       </c>
+      <c r="C14" t="s">
+        <v>390</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BGD</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
@@ -1669,6 +1778,13 @@
       <c r="B15" t="s">
         <v>29</v>
       </c>
+      <c r="C15" t="s">
+        <v>390</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BRB</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
@@ -1679,6 +1795,13 @@
       <c r="B16" t="s">
         <v>31</v>
       </c>
+      <c r="C16" t="s">
+        <v>390</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BLR</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
@@ -1689,6 +1812,13 @@
       <c r="B17" t="s">
         <v>33</v>
       </c>
+      <c r="C17" t="s">
+        <v>390</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BEL</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
@@ -1699,6 +1829,13 @@
       <c r="B18" t="s">
         <v>35</v>
       </c>
+      <c r="C18" t="s">
+        <v>390</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BLZ</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
@@ -1709,6 +1846,13 @@
       <c r="B19" t="s">
         <v>37</v>
       </c>
+      <c r="C19" t="s">
+        <v>390</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BEN</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
@@ -1719,6 +1863,13 @@
       <c r="B20" t="s">
         <v>39</v>
       </c>
+      <c r="C20" t="s">
+        <v>390</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BTN</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
@@ -1729,6 +1880,13 @@
       <c r="B21" t="s">
         <v>41</v>
       </c>
+      <c r="C21" t="s">
+        <v>390</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BOL</v>
+      </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
     </row>
@@ -1739,6 +1897,13 @@
       <c r="B22" t="s">
         <v>43</v>
       </c>
+      <c r="C22" t="s">
+        <v>390</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BIH</v>
+      </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
@@ -1749,6 +1914,13 @@
       <c r="B23" t="s">
         <v>45</v>
       </c>
+      <c r="C23" t="s">
+        <v>390</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BWA</v>
+      </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
@@ -1759,6 +1931,13 @@
       <c r="B24" t="s">
         <v>47</v>
       </c>
+      <c r="C24" t="s">
+        <v>390</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BRA</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
@@ -1769,6 +1948,13 @@
       <c r="B25" t="s">
         <v>49</v>
       </c>
+      <c r="C25" t="s">
+        <v>390</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BRN</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
@@ -1779,6 +1965,13 @@
       <c r="B26" t="s">
         <v>51</v>
       </c>
+      <c r="C26" t="s">
+        <v>390</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BGR</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
@@ -1789,6 +1982,13 @@
       <c r="B27" t="s">
         <v>53</v>
       </c>
+      <c r="C27" t="s">
+        <v>390</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BFA</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
@@ -1799,6 +1999,13 @@
       <c r="B28" t="s">
         <v>55</v>
       </c>
+      <c r="C28" t="s">
+        <v>390</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_BDI</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
@@ -1809,6 +2016,13 @@
       <c r="B29" t="s">
         <v>57</v>
       </c>
+      <c r="C29" t="s">
+        <v>390</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_KHM</v>
+      </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
     </row>
@@ -1819,6 +2033,13 @@
       <c r="B30" t="s">
         <v>59</v>
       </c>
+      <c r="C30" t="s">
+        <v>390</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_CMR</v>
+      </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
     </row>
@@ -1829,6 +2050,13 @@
       <c r="B31" t="s">
         <v>61</v>
       </c>
+      <c r="C31" t="s">
+        <v>390</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_CAN</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
@@ -1839,6 +2067,13 @@
       <c r="B32" t="s">
         <v>63</v>
       </c>
+      <c r="C32" t="s">
+        <v>390</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_CPV</v>
+      </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
@@ -1849,6 +2084,13 @@
       <c r="B33" t="s">
         <v>65</v>
       </c>
+      <c r="C33" t="s">
+        <v>390</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_CAF</v>
+      </c>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
@@ -1859,6 +2101,13 @@
       <c r="B34" t="s">
         <v>67</v>
       </c>
+      <c r="C34" t="s">
+        <v>390</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_TCD</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
@@ -1869,6 +2118,13 @@
       <c r="B35" t="s">
         <v>69</v>
       </c>
+      <c r="C35" t="s">
+        <v>390</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_CHL</v>
+      </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
@@ -1879,6 +2135,13 @@
       <c r="B36" t="s">
         <v>71</v>
       </c>
+      <c r="C36" t="s">
+        <v>390</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_CHN</v>
+      </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
@@ -1889,6 +2152,13 @@
       <c r="B37" t="s">
         <v>73</v>
       </c>
+      <c r="C37" t="s">
+        <v>390</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_COL</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
     </row>
@@ -1899,6 +2169,13 @@
       <c r="B38" t="s">
         <v>75</v>
       </c>
+      <c r="C38" t="s">
+        <v>390</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_COM</v>
+      </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
     </row>
@@ -1909,6 +2186,13 @@
       <c r="B39" t="s">
         <v>77</v>
       </c>
+      <c r="C39" t="s">
+        <v>390</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_COG</v>
+      </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
     </row>
@@ -1919,6 +2203,13 @@
       <c r="B40" t="s">
         <v>79</v>
       </c>
+      <c r="C40" t="s">
+        <v>390</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_COK</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
@@ -1929,6 +2220,13 @@
       <c r="B41" t="s">
         <v>81</v>
       </c>
+      <c r="C41" t="s">
+        <v>390</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_CRI</v>
+      </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
@@ -1939,6 +2237,13 @@
       <c r="B42" t="s">
         <v>83</v>
       </c>
+      <c r="C42" t="s">
+        <v>390</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_CIV</v>
+      </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
@@ -1949,6 +2254,13 @@
       <c r="B43" t="s">
         <v>85</v>
       </c>
+      <c r="C43" t="s">
+        <v>390</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_HRV</v>
+      </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
@@ -1959,6 +2271,13 @@
       <c r="B44" t="s">
         <v>87</v>
       </c>
+      <c r="C44" t="s">
+        <v>390</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_CUB</v>
+      </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
@@ -1969,6 +2288,13 @@
       <c r="B45" t="s">
         <v>89</v>
       </c>
+      <c r="C45" t="s">
+        <v>390</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_CYP</v>
+      </c>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
@@ -1979,6 +2305,13 @@
       <c r="B46" t="s">
         <v>91</v>
       </c>
+      <c r="C46" t="s">
+        <v>390</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_CZE</v>
+      </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
     </row>
@@ -1989,6 +2322,13 @@
       <c r="B47" t="s">
         <v>93</v>
       </c>
+      <c r="C47" t="s">
+        <v>390</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_PRK</v>
+      </c>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
     </row>
@@ -1999,6 +2339,13 @@
       <c r="B48" t="s">
         <v>95</v>
       </c>
+      <c r="C48" t="s">
+        <v>390</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_DNK</v>
+      </c>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
@@ -2009,6 +2356,13 @@
       <c r="B49" t="s">
         <v>97</v>
       </c>
+      <c r="C49" t="s">
+        <v>390</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_COD</v>
+      </c>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
@@ -2019,6 +2373,13 @@
       <c r="B50" t="s">
         <v>99</v>
       </c>
+      <c r="C50" t="s">
+        <v>390</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_DJI</v>
+      </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
@@ -2029,6 +2390,13 @@
       <c r="B51" t="s">
         <v>101</v>
       </c>
+      <c r="C51" t="s">
+        <v>390</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_DMA</v>
+      </c>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
@@ -2039,6 +2407,13 @@
       <c r="B52" t="s">
         <v>103</v>
       </c>
+      <c r="C52" t="s">
+        <v>390</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_DOM</v>
+      </c>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
@@ -2049,6 +2424,13 @@
       <c r="B53" t="s">
         <v>105</v>
       </c>
+      <c r="C53" t="s">
+        <v>390</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_ECU</v>
+      </c>
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
@@ -2059,6 +2441,13 @@
       <c r="B54" t="s">
         <v>107</v>
       </c>
+      <c r="C54" t="s">
+        <v>390</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_EGY</v>
+      </c>
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
@@ -2069,6 +2458,13 @@
       <c r="B55" t="s">
         <v>109</v>
       </c>
+      <c r="C55" t="s">
+        <v>390</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_SLV</v>
+      </c>
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
@@ -2079,6 +2475,13 @@
       <c r="B56" t="s">
         <v>111</v>
       </c>
+      <c r="C56" t="s">
+        <v>390</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_GNQ</v>
+      </c>
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
@@ -2089,6 +2492,13 @@
       <c r="B57" t="s">
         <v>113</v>
       </c>
+      <c r="C57" t="s">
+        <v>390</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_ERI</v>
+      </c>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
@@ -2099,6 +2509,13 @@
       <c r="B58" t="s">
         <v>115</v>
       </c>
+      <c r="C58" t="s">
+        <v>390</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_EST</v>
+      </c>
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
@@ -2109,6 +2526,13 @@
       <c r="B59" t="s">
         <v>117</v>
       </c>
+      <c r="C59" t="s">
+        <v>390</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_ETH</v>
+      </c>
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
@@ -2119,6 +2543,13 @@
       <c r="B60" t="s">
         <v>119</v>
       </c>
+      <c r="C60" t="s">
+        <v>390</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_FJI</v>
+      </c>
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
@@ -2129,6 +2560,13 @@
       <c r="B61" t="s">
         <v>121</v>
       </c>
+      <c r="C61" t="s">
+        <v>390</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_FIN</v>
+      </c>
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
@@ -2139,6 +2577,13 @@
       <c r="B62" t="s">
         <v>123</v>
       </c>
+      <c r="C62" t="s">
+        <v>390</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_FRA</v>
+      </c>
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
@@ -2149,6 +2594,13 @@
       <c r="B63" t="s">
         <v>125</v>
       </c>
+      <c r="C63" t="s">
+        <v>390</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_GAB</v>
+      </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
@@ -2159,6 +2611,13 @@
       <c r="B64" t="s">
         <v>127</v>
       </c>
+      <c r="C64" t="s">
+        <v>390</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_GMB</v>
+      </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>
@@ -2169,6 +2628,13 @@
       <c r="B65" t="s">
         <v>129</v>
       </c>
+      <c r="C65" t="s">
+        <v>390</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" si="0"/>
+        <v>UNAE/GVAKD_GEO</v>
+      </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
     </row>
@@ -2179,6 +2645,13 @@
       <c r="B66" t="s">
         <v>131</v>
       </c>
+      <c r="C66" t="s">
+        <v>390</v>
+      </c>
+      <c r="D66" t="str">
+        <f t="shared" ref="D66:D129" si="1">C66&amp;+B66</f>
+        <v>UNAE/GVAKD_DEU</v>
+      </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
     </row>
@@ -2189,6 +2662,13 @@
       <c r="B67" t="s">
         <v>133</v>
       </c>
+      <c r="C67" t="s">
+        <v>390</v>
+      </c>
+      <c r="D67" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_GHA</v>
+      </c>
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
@@ -2199,6 +2679,13 @@
       <c r="B68" t="s">
         <v>135</v>
       </c>
+      <c r="C68" t="s">
+        <v>390</v>
+      </c>
+      <c r="D68" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_GRC</v>
+      </c>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
@@ -2209,6 +2696,13 @@
       <c r="B69" t="s">
         <v>137</v>
       </c>
+      <c r="C69" t="s">
+        <v>390</v>
+      </c>
+      <c r="D69" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_GRD</v>
+      </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
@@ -2219,6 +2713,13 @@
       <c r="B70" t="s">
         <v>139</v>
       </c>
+      <c r="C70" t="s">
+        <v>390</v>
+      </c>
+      <c r="D70" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_GTM</v>
+      </c>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
@@ -2229,6 +2730,13 @@
       <c r="B71" t="s">
         <v>141</v>
       </c>
+      <c r="C71" t="s">
+        <v>390</v>
+      </c>
+      <c r="D71" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_GIN</v>
+      </c>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
@@ -2239,6 +2747,13 @@
       <c r="B72" t="s">
         <v>143</v>
       </c>
+      <c r="C72" t="s">
+        <v>390</v>
+      </c>
+      <c r="D72" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_GNB</v>
+      </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
@@ -2249,6 +2764,13 @@
       <c r="B73" t="s">
         <v>145</v>
       </c>
+      <c r="C73" t="s">
+        <v>390</v>
+      </c>
+      <c r="D73" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_GUY</v>
+      </c>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
     </row>
@@ -2259,6 +2781,13 @@
       <c r="B74" t="s">
         <v>147</v>
       </c>
+      <c r="C74" t="s">
+        <v>390</v>
+      </c>
+      <c r="D74" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_HTI</v>
+      </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
     </row>
@@ -2269,6 +2798,13 @@
       <c r="B75" t="s">
         <v>149</v>
       </c>
+      <c r="C75" t="s">
+        <v>390</v>
+      </c>
+      <c r="D75" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_HND</v>
+      </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
     </row>
@@ -2279,6 +2815,13 @@
       <c r="B76" t="s">
         <v>151</v>
       </c>
+      <c r="C76" t="s">
+        <v>390</v>
+      </c>
+      <c r="D76" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_HKG</v>
+      </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
@@ -2289,6 +2832,13 @@
       <c r="B77" t="s">
         <v>153</v>
       </c>
+      <c r="C77" t="s">
+        <v>390</v>
+      </c>
+      <c r="D77" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_HUN</v>
+      </c>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
@@ -2299,6 +2849,13 @@
       <c r="B78" t="s">
         <v>155</v>
       </c>
+      <c r="C78" t="s">
+        <v>390</v>
+      </c>
+      <c r="D78" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_ISL</v>
+      </c>
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
@@ -2309,6 +2866,13 @@
       <c r="B79" t="s">
         <v>157</v>
       </c>
+      <c r="C79" t="s">
+        <v>390</v>
+      </c>
+      <c r="D79" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_IND</v>
+      </c>
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
@@ -2319,6 +2883,13 @@
       <c r="B80" t="s">
         <v>159</v>
       </c>
+      <c r="C80" t="s">
+        <v>390</v>
+      </c>
+      <c r="D80" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_IDN</v>
+      </c>
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
@@ -2329,6 +2900,13 @@
       <c r="B81" t="s">
         <v>161</v>
       </c>
+      <c r="C81" t="s">
+        <v>390</v>
+      </c>
+      <c r="D81" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_IRN</v>
+      </c>
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
@@ -2339,6 +2917,13 @@
       <c r="B82" t="s">
         <v>163</v>
       </c>
+      <c r="C82" t="s">
+        <v>390</v>
+      </c>
+      <c r="D82" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_IRQ</v>
+      </c>
       <c r="H82" s="1"/>
       <c r="I82" s="1"/>
     </row>
@@ -2349,6 +2934,13 @@
       <c r="B83" t="s">
         <v>165</v>
       </c>
+      <c r="C83" t="s">
+        <v>390</v>
+      </c>
+      <c r="D83" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_IRL</v>
+      </c>
       <c r="H83" s="1"/>
       <c r="I83" s="1"/>
     </row>
@@ -2359,6 +2951,13 @@
       <c r="B84" t="s">
         <v>167</v>
       </c>
+      <c r="C84" t="s">
+        <v>390</v>
+      </c>
+      <c r="D84" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_ISR</v>
+      </c>
       <c r="H84" s="1"/>
       <c r="I84" s="1"/>
     </row>
@@ -2369,6 +2968,13 @@
       <c r="B85" t="s">
         <v>169</v>
       </c>
+      <c r="C85" t="s">
+        <v>390</v>
+      </c>
+      <c r="D85" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_ITA</v>
+      </c>
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
@@ -2379,6 +2985,13 @@
       <c r="B86" t="s">
         <v>171</v>
       </c>
+      <c r="C86" t="s">
+        <v>390</v>
+      </c>
+      <c r="D86" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_JAM</v>
+      </c>
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
@@ -2389,6 +3002,13 @@
       <c r="B87" t="s">
         <v>173</v>
       </c>
+      <c r="C87" t="s">
+        <v>390</v>
+      </c>
+      <c r="D87" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_JPN</v>
+      </c>
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
@@ -2399,6 +3019,13 @@
       <c r="B88" t="s">
         <v>175</v>
       </c>
+      <c r="C88" t="s">
+        <v>390</v>
+      </c>
+      <c r="D88" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_JOR</v>
+      </c>
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
@@ -2409,6 +3036,13 @@
       <c r="B89" t="s">
         <v>177</v>
       </c>
+      <c r="C89" t="s">
+        <v>390</v>
+      </c>
+      <c r="D89" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_KAZ</v>
+      </c>
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
@@ -2419,6 +3053,13 @@
       <c r="B90" t="s">
         <v>179</v>
       </c>
+      <c r="C90" t="s">
+        <v>390</v>
+      </c>
+      <c r="D90" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_KEN</v>
+      </c>
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
@@ -2429,6 +3070,13 @@
       <c r="B91" t="s">
         <v>181</v>
       </c>
+      <c r="C91" t="s">
+        <v>390</v>
+      </c>
+      <c r="D91" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_KIR</v>
+      </c>
       <c r="H91" s="1"/>
       <c r="I91" s="1"/>
     </row>
@@ -2439,6 +3087,13 @@
       <c r="B92" t="s">
         <v>183</v>
       </c>
+      <c r="C92" t="s">
+        <v>390</v>
+      </c>
+      <c r="D92" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_KWT</v>
+      </c>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
     </row>
@@ -2449,6 +3104,13 @@
       <c r="B93" t="s">
         <v>185</v>
       </c>
+      <c r="C93" t="s">
+        <v>390</v>
+      </c>
+      <c r="D93" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_KGZ</v>
+      </c>
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
     </row>
@@ -2459,6 +3121,13 @@
       <c r="B94" t="s">
         <v>187</v>
       </c>
+      <c r="C94" t="s">
+        <v>390</v>
+      </c>
+      <c r="D94" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_LAO</v>
+      </c>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
     </row>
@@ -2469,6 +3138,13 @@
       <c r="B95" t="s">
         <v>189</v>
       </c>
+      <c r="C95" t="s">
+        <v>390</v>
+      </c>
+      <c r="D95" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_LVA</v>
+      </c>
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
     </row>
@@ -2479,6 +3155,13 @@
       <c r="B96" t="s">
         <v>191</v>
       </c>
+      <c r="C96" t="s">
+        <v>390</v>
+      </c>
+      <c r="D96" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_LBN</v>
+      </c>
       <c r="H96" s="1"/>
       <c r="I96" s="1"/>
     </row>
@@ -2489,6 +3172,13 @@
       <c r="B97" t="s">
         <v>193</v>
       </c>
+      <c r="C97" t="s">
+        <v>390</v>
+      </c>
+      <c r="D97" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_LSO</v>
+      </c>
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
     </row>
@@ -2499,6 +3189,13 @@
       <c r="B98" t="s">
         <v>195</v>
       </c>
+      <c r="C98" t="s">
+        <v>390</v>
+      </c>
+      <c r="D98" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_LBR</v>
+      </c>
       <c r="H98" s="1"/>
       <c r="I98" s="1"/>
     </row>
@@ -2509,6 +3206,13 @@
       <c r="B99" t="s">
         <v>197</v>
       </c>
+      <c r="C99" t="s">
+        <v>390</v>
+      </c>
+      <c r="D99" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_LBY</v>
+      </c>
       <c r="H99" s="1"/>
       <c r="I99" s="1"/>
     </row>
@@ -2519,6 +3223,13 @@
       <c r="B100" t="s">
         <v>199</v>
       </c>
+      <c r="C100" t="s">
+        <v>390</v>
+      </c>
+      <c r="D100" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_LTU</v>
+      </c>
       <c r="H100" s="1"/>
       <c r="I100" s="1"/>
     </row>
@@ -2529,6 +3240,13 @@
       <c r="B101" t="s">
         <v>201</v>
       </c>
+      <c r="C101" t="s">
+        <v>390</v>
+      </c>
+      <c r="D101" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_LUX</v>
+      </c>
       <c r="H101" s="1"/>
       <c r="I101" s="1"/>
     </row>
@@ -2539,6 +3257,13 @@
       <c r="B102" t="s">
         <v>203</v>
       </c>
+      <c r="C102" t="s">
+        <v>390</v>
+      </c>
+      <c r="D102" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MDG</v>
+      </c>
       <c r="H102" s="1"/>
       <c r="I102" s="1"/>
     </row>
@@ -2549,6 +3274,13 @@
       <c r="B103" t="s">
         <v>205</v>
       </c>
+      <c r="C103" t="s">
+        <v>390</v>
+      </c>
+      <c r="D103" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MYS</v>
+      </c>
       <c r="H103" s="1"/>
       <c r="I103" s="1"/>
     </row>
@@ -2559,6 +3291,13 @@
       <c r="B104" t="s">
         <v>207</v>
       </c>
+      <c r="C104" t="s">
+        <v>390</v>
+      </c>
+      <c r="D104" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MDV</v>
+      </c>
       <c r="H104" s="1"/>
       <c r="I104" s="1"/>
     </row>
@@ -2569,6 +3308,13 @@
       <c r="B105" t="s">
         <v>209</v>
       </c>
+      <c r="C105" t="s">
+        <v>390</v>
+      </c>
+      <c r="D105" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MLT</v>
+      </c>
       <c r="H105" s="1"/>
       <c r="I105" s="1"/>
     </row>
@@ -2579,6 +3325,13 @@
       <c r="B106" t="s">
         <v>211</v>
       </c>
+      <c r="C106" t="s">
+        <v>390</v>
+      </c>
+      <c r="D106" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MHL</v>
+      </c>
       <c r="H106" s="1"/>
       <c r="I106" s="1"/>
     </row>
@@ -2589,6 +3342,13 @@
       <c r="B107" t="s">
         <v>213</v>
       </c>
+      <c r="C107" t="s">
+        <v>390</v>
+      </c>
+      <c r="D107" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MWI</v>
+      </c>
       <c r="H107" s="1"/>
       <c r="I107" s="1"/>
     </row>
@@ -2599,6 +3359,13 @@
       <c r="B108" t="s">
         <v>215</v>
       </c>
+      <c r="C108" t="s">
+        <v>390</v>
+      </c>
+      <c r="D108" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MRT</v>
+      </c>
       <c r="H108" s="1"/>
       <c r="I108" s="1"/>
     </row>
@@ -2609,6 +3376,13 @@
       <c r="B109" t="s">
         <v>217</v>
       </c>
+      <c r="C109" t="s">
+        <v>390</v>
+      </c>
+      <c r="D109" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MLI</v>
+      </c>
       <c r="H109" s="1"/>
       <c r="I109" s="1"/>
     </row>
@@ -2619,6 +3393,13 @@
       <c r="B110" t="s">
         <v>219</v>
       </c>
+      <c r="C110" t="s">
+        <v>390</v>
+      </c>
+      <c r="D110" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MUS</v>
+      </c>
       <c r="H110" s="1"/>
       <c r="I110" s="1"/>
     </row>
@@ -2629,6 +3410,13 @@
       <c r="B111" t="s">
         <v>221</v>
       </c>
+      <c r="C111" t="s">
+        <v>390</v>
+      </c>
+      <c r="D111" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MEX</v>
+      </c>
       <c r="H111" s="1"/>
       <c r="I111" s="1"/>
     </row>
@@ -2639,6 +3427,13 @@
       <c r="B112" t="s">
         <v>223</v>
       </c>
+      <c r="C112" t="s">
+        <v>390</v>
+      </c>
+      <c r="D112" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_FSM</v>
+      </c>
       <c r="H112" s="1"/>
       <c r="I112" s="1"/>
     </row>
@@ -2649,6 +3444,13 @@
       <c r="B113" t="s">
         <v>225</v>
       </c>
+      <c r="C113" t="s">
+        <v>390</v>
+      </c>
+      <c r="D113" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MCO</v>
+      </c>
       <c r="H113" s="1"/>
       <c r="I113" s="1"/>
     </row>
@@ -2659,6 +3461,13 @@
       <c r="B114" t="s">
         <v>227</v>
       </c>
+      <c r="C114" t="s">
+        <v>390</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MNG</v>
+      </c>
       <c r="H114" s="1"/>
       <c r="I114" s="1"/>
     </row>
@@ -2669,6 +3478,13 @@
       <c r="B115" t="s">
         <v>229</v>
       </c>
+      <c r="C115" t="s">
+        <v>390</v>
+      </c>
+      <c r="D115" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MNE</v>
+      </c>
       <c r="H115" s="1"/>
       <c r="I115" s="1"/>
     </row>
@@ -2679,6 +3495,13 @@
       <c r="B116" t="s">
         <v>231</v>
       </c>
+      <c r="C116" t="s">
+        <v>390</v>
+      </c>
+      <c r="D116" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MAR</v>
+      </c>
       <c r="H116" s="1"/>
       <c r="I116" s="1"/>
     </row>
@@ -2689,6 +3512,13 @@
       <c r="B117" t="s">
         <v>233</v>
       </c>
+      <c r="C117" t="s">
+        <v>390</v>
+      </c>
+      <c r="D117" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MOZ</v>
+      </c>
       <c r="H117" s="1"/>
       <c r="I117" s="1"/>
     </row>
@@ -2699,6 +3529,13 @@
       <c r="B118" t="s">
         <v>235</v>
       </c>
+      <c r="C118" t="s">
+        <v>390</v>
+      </c>
+      <c r="D118" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_MMR</v>
+      </c>
       <c r="H118" s="1"/>
       <c r="I118" s="1"/>
     </row>
@@ -2709,6 +3546,13 @@
       <c r="B119" t="s">
         <v>237</v>
       </c>
+      <c r="C119" t="s">
+        <v>390</v>
+      </c>
+      <c r="D119" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_NAM</v>
+      </c>
       <c r="H119" s="1"/>
       <c r="I119" s="1"/>
     </row>
@@ -2719,6 +3563,13 @@
       <c r="B120" t="s">
         <v>239</v>
       </c>
+      <c r="C120" t="s">
+        <v>390</v>
+      </c>
+      <c r="D120" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_NRU</v>
+      </c>
       <c r="H120" s="1"/>
       <c r="I120" s="1"/>
     </row>
@@ -2729,6 +3580,13 @@
       <c r="B121" t="s">
         <v>241</v>
       </c>
+      <c r="C121" t="s">
+        <v>390</v>
+      </c>
+      <c r="D121" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_NPL</v>
+      </c>
       <c r="H121" s="1"/>
       <c r="I121" s="1"/>
     </row>
@@ -2739,6 +3597,13 @@
       <c r="B122" t="s">
         <v>243</v>
       </c>
+      <c r="C122" t="s">
+        <v>390</v>
+      </c>
+      <c r="D122" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_NLD</v>
+      </c>
       <c r="H122" s="1"/>
       <c r="I122" s="1"/>
     </row>
@@ -2749,6 +3614,13 @@
       <c r="B123" t="s">
         <v>245</v>
       </c>
+      <c r="C123" t="s">
+        <v>390</v>
+      </c>
+      <c r="D123" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_NZL</v>
+      </c>
       <c r="H123" s="1"/>
       <c r="I123" s="1"/>
     </row>
@@ -2759,6 +3631,13 @@
       <c r="B124" t="s">
         <v>247</v>
       </c>
+      <c r="C124" t="s">
+        <v>390</v>
+      </c>
+      <c r="D124" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_NIC</v>
+      </c>
       <c r="H124" s="1"/>
       <c r="I124" s="1"/>
     </row>
@@ -2769,6 +3648,13 @@
       <c r="B125" t="s">
         <v>249</v>
       </c>
+      <c r="C125" t="s">
+        <v>390</v>
+      </c>
+      <c r="D125" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_NER</v>
+      </c>
       <c r="H125" s="1"/>
       <c r="I125" s="1"/>
     </row>
@@ -2779,6 +3665,13 @@
       <c r="B126" t="s">
         <v>251</v>
       </c>
+      <c r="C126" t="s">
+        <v>390</v>
+      </c>
+      <c r="D126" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_NGA</v>
+      </c>
       <c r="H126" s="1"/>
       <c r="I126" s="1"/>
     </row>
@@ -2789,6 +3682,13 @@
       <c r="B127" t="s">
         <v>253</v>
       </c>
+      <c r="C127" t="s">
+        <v>390</v>
+      </c>
+      <c r="D127" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_NIU</v>
+      </c>
       <c r="H127" s="1"/>
       <c r="I127" s="1"/>
     </row>
@@ -2799,6 +3699,13 @@
       <c r="B128" t="s">
         <v>255</v>
       </c>
+      <c r="C128" t="s">
+        <v>390</v>
+      </c>
+      <c r="D128" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_NOR</v>
+      </c>
       <c r="H128" s="1"/>
       <c r="I128" s="1"/>
     </row>
@@ -2809,6 +3716,13 @@
       <c r="B129" t="s">
         <v>257</v>
       </c>
+      <c r="C129" t="s">
+        <v>390</v>
+      </c>
+      <c r="D129" t="str">
+        <f t="shared" si="1"/>
+        <v>UNAE/GVAKD_OMN</v>
+      </c>
       <c r="H129" s="1"/>
       <c r="I129" s="1"/>
     </row>
@@ -2819,6 +3733,13 @@
       <c r="B130" t="s">
         <v>259</v>
       </c>
+      <c r="C130" t="s">
+        <v>390</v>
+      </c>
+      <c r="D130" t="str">
+        <f t="shared" ref="D130:D193" si="2">C130&amp;+B130</f>
+        <v>UNAE/GVAKD_PAK</v>
+      </c>
       <c r="H130" s="1"/>
       <c r="I130" s="1"/>
     </row>
@@ -2829,6 +3750,13 @@
       <c r="B131" t="s">
         <v>261</v>
       </c>
+      <c r="C131" t="s">
+        <v>390</v>
+      </c>
+      <c r="D131" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_PLW</v>
+      </c>
       <c r="H131" s="1"/>
       <c r="I131" s="1"/>
     </row>
@@ -2839,6 +3767,13 @@
       <c r="B132" t="s">
         <v>263</v>
       </c>
+      <c r="C132" t="s">
+        <v>390</v>
+      </c>
+      <c r="D132" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_PAN</v>
+      </c>
       <c r="H132" s="1"/>
       <c r="I132" s="1"/>
     </row>
@@ -2849,6 +3784,13 @@
       <c r="B133" t="s">
         <v>265</v>
       </c>
+      <c r="C133" t="s">
+        <v>390</v>
+      </c>
+      <c r="D133" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_PNG</v>
+      </c>
       <c r="H133" s="1"/>
       <c r="I133" s="1"/>
     </row>
@@ -2859,6 +3801,13 @@
       <c r="B134" t="s">
         <v>267</v>
       </c>
+      <c r="C134" t="s">
+        <v>390</v>
+      </c>
+      <c r="D134" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_PRY</v>
+      </c>
       <c r="H134" s="1"/>
       <c r="I134" s="1"/>
     </row>
@@ -2869,6 +3818,13 @@
       <c r="B135" t="s">
         <v>269</v>
       </c>
+      <c r="C135" t="s">
+        <v>390</v>
+      </c>
+      <c r="D135" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_PER</v>
+      </c>
       <c r="H135" s="1"/>
       <c r="I135" s="1"/>
     </row>
@@ -2879,6 +3835,13 @@
       <c r="B136" t="s">
         <v>271</v>
       </c>
+      <c r="C136" t="s">
+        <v>390</v>
+      </c>
+      <c r="D136" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_PHL</v>
+      </c>
       <c r="H136" s="1"/>
       <c r="I136" s="1"/>
     </row>
@@ -2889,6 +3852,13 @@
       <c r="B137" t="s">
         <v>273</v>
       </c>
+      <c r="C137" t="s">
+        <v>390</v>
+      </c>
+      <c r="D137" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_POL</v>
+      </c>
       <c r="H137" s="1"/>
       <c r="I137" s="1"/>
     </row>
@@ -2899,6 +3869,13 @@
       <c r="B138" t="s">
         <v>275</v>
       </c>
+      <c r="C138" t="s">
+        <v>390</v>
+      </c>
+      <c r="D138" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_PRT</v>
+      </c>
       <c r="H138" s="1"/>
       <c r="I138" s="1"/>
     </row>
@@ -2909,6 +3886,13 @@
       <c r="B139" t="s">
         <v>277</v>
       </c>
+      <c r="C139" t="s">
+        <v>390</v>
+      </c>
+      <c r="D139" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_QAT</v>
+      </c>
       <c r="H139" s="1"/>
       <c r="I139" s="1"/>
     </row>
@@ -2919,6 +3903,13 @@
       <c r="B140" t="s">
         <v>279</v>
       </c>
+      <c r="C140" t="s">
+        <v>390</v>
+      </c>
+      <c r="D140" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_KOR</v>
+      </c>
       <c r="H140" s="1"/>
       <c r="I140" s="1"/>
     </row>
@@ -2929,6 +3920,13 @@
       <c r="B141" t="s">
         <v>281</v>
       </c>
+      <c r="C141" t="s">
+        <v>390</v>
+      </c>
+      <c r="D141" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_MDA</v>
+      </c>
       <c r="H141" s="1"/>
       <c r="I141" s="1"/>
     </row>
@@ -2939,6 +3937,13 @@
       <c r="B142" t="s">
         <v>283</v>
       </c>
+      <c r="C142" t="s">
+        <v>390</v>
+      </c>
+      <c r="D142" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_ROU</v>
+      </c>
       <c r="H142" s="1"/>
       <c r="I142" s="1"/>
     </row>
@@ -2949,6 +3954,13 @@
       <c r="B143" t="s">
         <v>285</v>
       </c>
+      <c r="C143" t="s">
+        <v>390</v>
+      </c>
+      <c r="D143" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_RUS</v>
+      </c>
       <c r="H143" s="1"/>
       <c r="I143" s="1"/>
     </row>
@@ -2959,6 +3971,13 @@
       <c r="B144" t="s">
         <v>287</v>
       </c>
+      <c r="C144" t="s">
+        <v>390</v>
+      </c>
+      <c r="D144" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_RWA</v>
+      </c>
       <c r="H144" s="1"/>
       <c r="I144" s="1"/>
     </row>
@@ -2969,6 +3988,13 @@
       <c r="B145" t="s">
         <v>289</v>
       </c>
+      <c r="C145" t="s">
+        <v>390</v>
+      </c>
+      <c r="D145" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_KNA</v>
+      </c>
       <c r="H145" s="1"/>
       <c r="I145" s="1"/>
     </row>
@@ -2979,6 +4005,13 @@
       <c r="B146" t="s">
         <v>291</v>
       </c>
+      <c r="C146" t="s">
+        <v>390</v>
+      </c>
+      <c r="D146" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_LCA</v>
+      </c>
       <c r="H146" s="1"/>
       <c r="I146" s="1"/>
     </row>
@@ -2989,6 +4022,13 @@
       <c r="B147" t="s">
         <v>293</v>
       </c>
+      <c r="C147" t="s">
+        <v>390</v>
+      </c>
+      <c r="D147" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_VCT</v>
+      </c>
       <c r="H147" s="1"/>
       <c r="I147" s="1"/>
     </row>
@@ -2999,6 +4039,13 @@
       <c r="B148" t="s">
         <v>295</v>
       </c>
+      <c r="C148" t="s">
+        <v>390</v>
+      </c>
+      <c r="D148" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_WSM</v>
+      </c>
       <c r="H148" s="1"/>
       <c r="I148" s="1"/>
     </row>
@@ -3009,6 +4056,13 @@
       <c r="B149" t="s">
         <v>297</v>
       </c>
+      <c r="C149" t="s">
+        <v>390</v>
+      </c>
+      <c r="D149" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SMR</v>
+      </c>
       <c r="H149" s="1"/>
       <c r="I149" s="1"/>
     </row>
@@ -3019,6 +4073,13 @@
       <c r="B150" t="s">
         <v>299</v>
       </c>
+      <c r="C150" t="s">
+        <v>390</v>
+      </c>
+      <c r="D150" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_STP</v>
+      </c>
       <c r="H150" s="1"/>
       <c r="I150" s="1"/>
     </row>
@@ -3029,6 +4090,13 @@
       <c r="B151" t="s">
         <v>301</v>
       </c>
+      <c r="C151" t="s">
+        <v>390</v>
+      </c>
+      <c r="D151" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SAU</v>
+      </c>
       <c r="H151" s="1"/>
       <c r="I151" s="1"/>
     </row>
@@ -3039,6 +4107,13 @@
       <c r="B152" t="s">
         <v>303</v>
       </c>
+      <c r="C152" t="s">
+        <v>390</v>
+      </c>
+      <c r="D152" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SEN</v>
+      </c>
       <c r="H152" s="1"/>
       <c r="I152" s="1"/>
     </row>
@@ -3049,6 +4124,13 @@
       <c r="B153" t="s">
         <v>305</v>
       </c>
+      <c r="C153" t="s">
+        <v>390</v>
+      </c>
+      <c r="D153" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SRB</v>
+      </c>
       <c r="H153" s="1"/>
       <c r="I153" s="1"/>
     </row>
@@ -3059,6 +4141,13 @@
       <c r="B154" t="s">
         <v>307</v>
       </c>
+      <c r="C154" t="s">
+        <v>390</v>
+      </c>
+      <c r="D154" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SYC</v>
+      </c>
       <c r="H154" s="1"/>
       <c r="I154" s="1"/>
     </row>
@@ -3069,6 +4158,13 @@
       <c r="B155" t="s">
         <v>309</v>
       </c>
+      <c r="C155" t="s">
+        <v>390</v>
+      </c>
+      <c r="D155" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SLE</v>
+      </c>
       <c r="H155" s="1"/>
       <c r="I155" s="1"/>
     </row>
@@ -3079,6 +4175,13 @@
       <c r="B156" t="s">
         <v>311</v>
       </c>
+      <c r="C156" t="s">
+        <v>390</v>
+      </c>
+      <c r="D156" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SGP</v>
+      </c>
       <c r="H156" s="1"/>
       <c r="I156" s="1"/>
     </row>
@@ -3089,6 +4192,13 @@
       <c r="B157" t="s">
         <v>313</v>
       </c>
+      <c r="C157" t="s">
+        <v>390</v>
+      </c>
+      <c r="D157" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SVK</v>
+      </c>
       <c r="H157" s="1"/>
       <c r="I157" s="1"/>
     </row>
@@ -3099,6 +4209,13 @@
       <c r="B158" t="s">
         <v>315</v>
       </c>
+      <c r="C158" t="s">
+        <v>390</v>
+      </c>
+      <c r="D158" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SVN</v>
+      </c>
       <c r="H158" s="1"/>
       <c r="I158" s="1"/>
     </row>
@@ -3109,6 +4226,13 @@
       <c r="B159" t="s">
         <v>317</v>
       </c>
+      <c r="C159" t="s">
+        <v>390</v>
+      </c>
+      <c r="D159" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SLB</v>
+      </c>
       <c r="H159" s="1"/>
       <c r="I159" s="1"/>
     </row>
@@ -3119,6 +4243,13 @@
       <c r="B160" t="s">
         <v>319</v>
       </c>
+      <c r="C160" t="s">
+        <v>390</v>
+      </c>
+      <c r="D160" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SOM</v>
+      </c>
       <c r="H160" s="1"/>
       <c r="I160" s="1"/>
     </row>
@@ -3129,6 +4260,13 @@
       <c r="B161" t="s">
         <v>321</v>
       </c>
+      <c r="C161" t="s">
+        <v>390</v>
+      </c>
+      <c r="D161" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_ZAF</v>
+      </c>
       <c r="H161" s="1"/>
       <c r="I161" s="1"/>
     </row>
@@ -3139,6 +4277,13 @@
       <c r="B162" t="s">
         <v>323</v>
       </c>
+      <c r="C162" t="s">
+        <v>390</v>
+      </c>
+      <c r="D162" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SSD</v>
+      </c>
       <c r="H162" s="1"/>
       <c r="I162" s="1"/>
     </row>
@@ -3149,6 +4294,13 @@
       <c r="B163" t="s">
         <v>325</v>
       </c>
+      <c r="C163" t="s">
+        <v>390</v>
+      </c>
+      <c r="D163" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_ESP</v>
+      </c>
       <c r="H163" s="1"/>
       <c r="I163" s="1"/>
     </row>
@@ -3159,6 +4311,13 @@
       <c r="B164" t="s">
         <v>327</v>
       </c>
+      <c r="C164" t="s">
+        <v>390</v>
+      </c>
+      <c r="D164" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_LKA</v>
+      </c>
       <c r="H164" s="1"/>
       <c r="I164" s="1"/>
     </row>
@@ -3169,6 +4328,13 @@
       <c r="B165" t="s">
         <v>329</v>
       </c>
+      <c r="C165" t="s">
+        <v>390</v>
+      </c>
+      <c r="D165" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SDN</v>
+      </c>
       <c r="H165" s="1"/>
       <c r="I165" s="1"/>
     </row>
@@ -3179,6 +4345,13 @@
       <c r="B166" t="s">
         <v>331</v>
       </c>
+      <c r="C166" t="s">
+        <v>390</v>
+      </c>
+      <c r="D166" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SUR</v>
+      </c>
       <c r="H166" s="1"/>
       <c r="I166" s="1"/>
     </row>
@@ -3189,6 +4362,13 @@
       <c r="B167" t="s">
         <v>333</v>
       </c>
+      <c r="C167" t="s">
+        <v>390</v>
+      </c>
+      <c r="D167" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SWZ</v>
+      </c>
       <c r="H167" s="1"/>
       <c r="I167" s="1"/>
     </row>
@@ -3199,6 +4379,13 @@
       <c r="B168" t="s">
         <v>335</v>
       </c>
+      <c r="C168" t="s">
+        <v>390</v>
+      </c>
+      <c r="D168" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SWE</v>
+      </c>
       <c r="H168" s="1"/>
       <c r="I168" s="1"/>
     </row>
@@ -3209,6 +4396,13 @@
       <c r="B169" t="s">
         <v>337</v>
       </c>
+      <c r="C169" t="s">
+        <v>390</v>
+      </c>
+      <c r="D169" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_CHE</v>
+      </c>
       <c r="H169" s="1"/>
       <c r="I169" s="1"/>
     </row>
@@ -3219,6 +4413,13 @@
       <c r="B170" t="s">
         <v>339</v>
       </c>
+      <c r="C170" t="s">
+        <v>390</v>
+      </c>
+      <c r="D170" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_SYR</v>
+      </c>
       <c r="H170" s="1"/>
       <c r="I170" s="1"/>
     </row>
@@ -3229,6 +4430,13 @@
       <c r="B171" t="s">
         <v>341</v>
       </c>
+      <c r="C171" t="s">
+        <v>390</v>
+      </c>
+      <c r="D171" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_TJK</v>
+      </c>
       <c r="H171" s="1"/>
       <c r="I171" s="1"/>
     </row>
@@ -3239,6 +4447,13 @@
       <c r="B172" t="s">
         <v>343</v>
       </c>
+      <c r="C172" t="s">
+        <v>390</v>
+      </c>
+      <c r="D172" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_THA</v>
+      </c>
       <c r="H172" s="1"/>
       <c r="I172" s="1"/>
     </row>
@@ -3249,6 +4464,13 @@
       <c r="B173" t="s">
         <v>345</v>
       </c>
+      <c r="C173" t="s">
+        <v>390</v>
+      </c>
+      <c r="D173" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_MKD</v>
+      </c>
       <c r="H173" s="1"/>
       <c r="I173" s="1"/>
     </row>
@@ -3259,6 +4481,13 @@
       <c r="B174" t="s">
         <v>347</v>
       </c>
+      <c r="C174" t="s">
+        <v>390</v>
+      </c>
+      <c r="D174" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_TLS</v>
+      </c>
       <c r="H174" s="1"/>
       <c r="I174" s="1"/>
     </row>
@@ -3269,6 +4498,13 @@
       <c r="B175" t="s">
         <v>349</v>
       </c>
+      <c r="C175" t="s">
+        <v>390</v>
+      </c>
+      <c r="D175" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_TGO</v>
+      </c>
       <c r="H175" s="1"/>
       <c r="I175" s="1"/>
     </row>
@@ -3279,6 +4515,13 @@
       <c r="B176" t="s">
         <v>351</v>
       </c>
+      <c r="C176" t="s">
+        <v>390</v>
+      </c>
+      <c r="D176" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_TON</v>
+      </c>
       <c r="H176" s="1"/>
       <c r="I176" s="1"/>
     </row>
@@ -3289,6 +4532,13 @@
       <c r="B177" t="s">
         <v>353</v>
       </c>
+      <c r="C177" t="s">
+        <v>390</v>
+      </c>
+      <c r="D177" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_TTO</v>
+      </c>
       <c r="H177" s="1"/>
       <c r="I177" s="1"/>
     </row>
@@ -3299,6 +4549,13 @@
       <c r="B178" t="s">
         <v>355</v>
       </c>
+      <c r="C178" t="s">
+        <v>390</v>
+      </c>
+      <c r="D178" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_TUN</v>
+      </c>
       <c r="H178" s="1"/>
       <c r="I178" s="1"/>
     </row>
@@ -3309,6 +4566,13 @@
       <c r="B179" t="s">
         <v>357</v>
       </c>
+      <c r="C179" t="s">
+        <v>390</v>
+      </c>
+      <c r="D179" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_TUR</v>
+      </c>
       <c r="H179" s="1"/>
       <c r="I179" s="1"/>
     </row>
@@ -3319,6 +4583,13 @@
       <c r="B180" t="s">
         <v>359</v>
       </c>
+      <c r="C180" t="s">
+        <v>390</v>
+      </c>
+      <c r="D180" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_TKM</v>
+      </c>
       <c r="H180" s="1"/>
       <c r="I180" s="1"/>
     </row>
@@ -3329,6 +4600,13 @@
       <c r="B181" t="s">
         <v>361</v>
       </c>
+      <c r="C181" t="s">
+        <v>390</v>
+      </c>
+      <c r="D181" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_TUV</v>
+      </c>
       <c r="H181" s="1"/>
       <c r="I181" s="1"/>
     </row>
@@ -3339,6 +4617,13 @@
       <c r="B182" t="s">
         <v>363</v>
       </c>
+      <c r="C182" t="s">
+        <v>390</v>
+      </c>
+      <c r="D182" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_UGA</v>
+      </c>
       <c r="H182" s="1"/>
       <c r="I182" s="1"/>
     </row>
@@ -3349,6 +4634,13 @@
       <c r="B183" t="s">
         <v>365</v>
       </c>
+      <c r="C183" t="s">
+        <v>390</v>
+      </c>
+      <c r="D183" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_UKR</v>
+      </c>
       <c r="H183" s="1"/>
       <c r="I183" s="1"/>
     </row>
@@ -3359,6 +4651,13 @@
       <c r="B184" t="s">
         <v>367</v>
       </c>
+      <c r="C184" t="s">
+        <v>390</v>
+      </c>
+      <c r="D184" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_ARE</v>
+      </c>
       <c r="H184" s="1"/>
       <c r="I184" s="1"/>
     </row>
@@ -3369,6 +4668,13 @@
       <c r="B185" t="s">
         <v>369</v>
       </c>
+      <c r="C185" t="s">
+        <v>390</v>
+      </c>
+      <c r="D185" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_GBR</v>
+      </c>
       <c r="H185" s="1"/>
       <c r="I185" s="1"/>
     </row>
@@ -3379,6 +4685,13 @@
       <c r="B186" t="s">
         <v>371</v>
       </c>
+      <c r="C186" t="s">
+        <v>390</v>
+      </c>
+      <c r="D186" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_TZA</v>
+      </c>
       <c r="H186" s="1"/>
       <c r="I186" s="1"/>
     </row>
@@ -3389,6 +4702,13 @@
       <c r="B187" t="s">
         <v>373</v>
       </c>
+      <c r="C187" t="s">
+        <v>390</v>
+      </c>
+      <c r="D187" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_USA</v>
+      </c>
       <c r="H187" s="1"/>
       <c r="I187" s="1"/>
     </row>
@@ -3399,6 +4719,13 @@
       <c r="B188" t="s">
         <v>375</v>
       </c>
+      <c r="C188" t="s">
+        <v>390</v>
+      </c>
+      <c r="D188" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_URY</v>
+      </c>
       <c r="H188" s="1"/>
       <c r="I188" s="1"/>
     </row>
@@ -3409,6 +4736,13 @@
       <c r="B189" t="s">
         <v>377</v>
       </c>
+      <c r="C189" t="s">
+        <v>390</v>
+      </c>
+      <c r="D189" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_UZB</v>
+      </c>
       <c r="H189" s="1"/>
       <c r="I189" s="1"/>
     </row>
@@ -3419,6 +4753,13 @@
       <c r="B190" t="s">
         <v>379</v>
       </c>
+      <c r="C190" t="s">
+        <v>390</v>
+      </c>
+      <c r="D190" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_VUT</v>
+      </c>
       <c r="H190" s="1"/>
       <c r="I190" s="1"/>
     </row>
@@ -3429,6 +4770,13 @@
       <c r="B191" t="s">
         <v>381</v>
       </c>
+      <c r="C191" t="s">
+        <v>390</v>
+      </c>
+      <c r="D191" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_VEN</v>
+      </c>
       <c r="H191" s="1"/>
       <c r="I191" s="1"/>
     </row>
@@ -3439,6 +4787,13 @@
       <c r="B192" t="s">
         <v>383</v>
       </c>
+      <c r="C192" t="s">
+        <v>390</v>
+      </c>
+      <c r="D192" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_VNM</v>
+      </c>
       <c r="H192" s="1"/>
       <c r="I192" s="1"/>
     </row>
@@ -3449,6 +4804,13 @@
       <c r="B193" t="s">
         <v>385</v>
       </c>
+      <c r="C193" t="s">
+        <v>390</v>
+      </c>
+      <c r="D193" t="str">
+        <f t="shared" si="2"/>
+        <v>UNAE/GVAKD_YEM</v>
+      </c>
       <c r="H193" s="1"/>
       <c r="I193" s="1"/>
     </row>
@@ -3459,6 +4821,13 @@
       <c r="B194" t="s">
         <v>387</v>
       </c>
+      <c r="C194" t="s">
+        <v>390</v>
+      </c>
+      <c r="D194" t="str">
+        <f t="shared" ref="D194:D195" si="3">C194&amp;+B194</f>
+        <v>UNAE/GVAKD_ZMB</v>
+      </c>
       <c r="H194" s="1"/>
       <c r="I194" s="1"/>
     </row>
@@ -3468,6 +4837,13 @@
       </c>
       <c r="B195" t="s">
         <v>389</v>
+      </c>
+      <c r="C195" t="s">
+        <v>390</v>
+      </c>
+      <c r="D195" t="str">
+        <f t="shared" si="3"/>
+        <v>UNAE/GVAKD_ZWE</v>
       </c>
       <c r="H195" s="1"/>
       <c r="I195" s="1"/>

</xml_diff>